<commit_message>
Added Tier 1 experiment conversion time
</commit_message>
<xml_diff>
--- a/Docs/Station Science List.xlsx
+++ b/Docs/Station Science List.xlsx
@@ -13,7 +13,7 @@
     <sheet name="Lab Modules" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Experiments and Notes'!$A$1:$V$23</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Experiments and Notes'!$A$1:$X$23</definedName>
     <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">'Lab Modules'!$A$1:$G$11</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="186">
   <si>
     <t xml:space="preserve">Experiment No.:</t>
   </si>
@@ -93,6 +93,12 @@
   </si>
   <si>
     <t xml:space="preserve">Solutions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kerbin Days</t>
   </si>
   <si>
     <t xml:space="preserve">Research Lab</t>
@@ -741,13 +747,13 @@
     <t xml:space="preserve">Resource Storage</t>
   </si>
   <si>
-    <t xml:space="preserve">Input 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Input 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Output</t>
+    <t xml:space="preserve">Input 1 (p/second)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Input 2 (p/second)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Output (p/second)</t>
   </si>
   <si>
     <t xml:space="preserve">StnSciLab</t>
@@ -868,8 +874,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="167" formatCode="0"/>
   </numFmts>
   <fonts count="31">
     <font>
@@ -934,6 +943,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -1085,13 +1101,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="6"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
   </fonts>
   <fills count="13">
     <fill>
@@ -1234,11 +1243,11 @@
     <xf numFmtId="164" fontId="9" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="65">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1255,6 +1264,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="24" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1299,7 +1312,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="6" borderId="0" xfId="29" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="6" borderId="0" xfId="29" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1319,7 +1344,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1327,16 +1352,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1351,7 +1372,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1359,27 +1380,31 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1395,7 +1420,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="30" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1407,7 +1432,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="30" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1423,7 +1448,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="30" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1435,7 +1460,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="30" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1463,7 +1488,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="30" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1479,7 +1504,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="30" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1691,9 +1716,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>2026440</xdr:colOff>
+      <xdr:colOff>2026080</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>163800</xdr:rowOff>
+      <xdr:rowOff>163440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1702,8 +1727,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="98280" y="5989320"/>
-          <a:ext cx="4790160" cy="2586960"/>
+          <a:off x="98280" y="2834640"/>
+          <a:ext cx="4789800" cy="2586600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1850,10 +1875,10 @@
       <xdr:rowOff>153000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>658440</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>658080</xdr:colOff>
       <xdr:row>73</xdr:row>
-      <xdr:rowOff>1800</xdr:rowOff>
+      <xdr:rowOff>1440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1862,8 +1887,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5398200" y="11720160"/>
-          <a:ext cx="7936200" cy="1075680"/>
+          <a:off x="5398200" y="8565480"/>
+          <a:ext cx="9408240" cy="1075320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1999,16 +2024,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>556200</xdr:colOff>
       <xdr:row>50</xdr:row>
       <xdr:rowOff>152280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>2410200</xdr:colOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>2409840</xdr:colOff>
       <xdr:row>61</xdr:row>
-      <xdr:rowOff>85680</xdr:rowOff>
+      <xdr:rowOff>85320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2017,8 +2042,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13232160" y="8915400"/>
-          <a:ext cx="7958160" cy="1861200"/>
+          <a:off x="14704560" y="5760720"/>
+          <a:ext cx="7957800" cy="1860840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2139,9 +2164,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>788760</xdr:colOff>
+      <xdr:colOff>788400</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>84240</xdr:rowOff>
+      <xdr:rowOff>83880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2150,8 +2175,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="599040" y="4779360"/>
-          <a:ext cx="3051720" cy="913320"/>
+          <a:off x="599040" y="1624680"/>
+          <a:ext cx="3051360" cy="912960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2313,9 +2338,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1505520</xdr:colOff>
+      <xdr:colOff>1505160</xdr:colOff>
       <xdr:row>57</xdr:row>
-      <xdr:rowOff>60480</xdr:rowOff>
+      <xdr:rowOff>60120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2324,8 +2349,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="220320" y="8857440"/>
-          <a:ext cx="4147200" cy="1193040"/>
+          <a:off x="220320" y="5702760"/>
+          <a:ext cx="4146840" cy="1192680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2578,9 +2603,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1585800</xdr:colOff>
+      <xdr:colOff>1585440</xdr:colOff>
       <xdr:row>82</xdr:row>
-      <xdr:rowOff>167400</xdr:rowOff>
+      <xdr:rowOff>167040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2589,8 +2614,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="181800" y="10212120"/>
-          <a:ext cx="4266000" cy="4326480"/>
+          <a:off x="181800" y="7057440"/>
+          <a:ext cx="4265640" cy="4326120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3184,14 +3209,14 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>158040</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>13680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>447120</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>54000</xdr:rowOff>
+      <xdr:colOff>446760</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>53640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3201,7 +3226,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="8411040" y="4219920"/>
-          <a:ext cx="4712040" cy="3019680"/>
+          <a:ext cx="4711680" cy="3019320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3498,15 +3523,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>87120</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:colOff>463680</xdr:colOff>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>114840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>67680</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>144360</xdr:rowOff>
+      <xdr:colOff>697680</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>144000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3516,7 +3541,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="13799160" y="4145760"/>
-          <a:ext cx="3977280" cy="2483280"/>
+          <a:ext cx="3976920" cy="2482920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3695,14 +3720,14 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>292320</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>106200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>677160</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>46800</xdr:rowOff>
+      <xdr:colOff>676800</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>46440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3712,7 +3737,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5261040" y="4137120"/>
-          <a:ext cx="2954880" cy="4146840"/>
+          <a:ext cx="2954520" cy="4146480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3998,9 +4023,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>408240</xdr:colOff>
+      <xdr:colOff>407880</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>96840</xdr:rowOff>
+      <xdr:rowOff>96480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4010,7 +4035,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="115560" y="1352880"/>
-          <a:ext cx="7619400" cy="7169760"/>
+          <a:ext cx="7620120" cy="7169400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4348,16 +4373,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>352440</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>87120</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1028520</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>25560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>6587640</xdr:colOff>
+      <xdr:colOff>5839200</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>154800</xdr:rowOff>
+      <xdr:rowOff>39600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4366,8 +4391,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9142920" y="3566880"/>
-          <a:ext cx="6235200" cy="2993760"/>
+          <a:off x="9162360" y="3706200"/>
+          <a:ext cx="6234840" cy="2993400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4399,7 +4424,7 @@
             <a:rPr b="0" lang="en-GB" sz="1200" spc="-1" strike="noStrike">
               <a:latin typeface="Times New Roman"/>
             </a:rPr>
-            <a:t>0.00027777777 = 1 unit per hour of game time</a:t>
+            <a:t>0.00027777777 = per second</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-GB" sz="1200" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
@@ -4425,8 +4450,78 @@
             <a:rPr b="0" lang="en-GB" sz="1200" spc="-1" strike="noStrike">
               <a:latin typeface="Times New Roman"/>
             </a:rPr>
-            <a:t>Numbers need to change!</a:t>
-          </a:r>
+            <a:t>0.0166666662 = per minute</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="en-GB" sz="1200" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:endParaRPr b="0" lang="en-GB" sz="1200" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="en-GB" sz="1200" spc="-1" strike="noStrike">
+              <a:latin typeface="Times New Roman"/>
+            </a:rPr>
+            <a:t>0.999999972 = per hour</a:t>
+          </a:r>
+          <a:br/>
+          <a:br/>
+          <a:r>
+            <a:rPr b="0" lang="en-GB" sz="1200" spc="-1" strike="noStrike">
+              <a:latin typeface="Times New Roman"/>
+            </a:rPr>
+            <a:t>3.999999888 = per Kerbin day (4 hours)</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="en-GB" sz="1200" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:endParaRPr b="0" lang="en-GB" sz="1200" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="en-GB" sz="1200" spc="-1" strike="noStrike">
+              <a:latin typeface="Times New Roman"/>
+            </a:rPr>
+            <a:t>1 unit per hour conversion rates ^^^^</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="en-GB" sz="1200" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
           <a:endParaRPr b="0" lang="en-GB" sz="1200" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
           </a:endParaRPr>
@@ -4450,18 +4545,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
+  <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:V64"/>
+  <dimension ref="A1:X64"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="4" ySplit="0" topLeftCell="E1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="J17" activeCellId="0" sqref="J17"/>
+      <selection pane="topRight" activeCell="P31" activeCellId="0" sqref="P31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.01953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.85"/>
@@ -4476,14 +4571,16 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="16.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="14.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="12.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="14.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="13.7"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="17" min="17" style="0" width="16.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="13.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="13.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="15.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="15.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="88.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="9.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="14.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="13.7"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="19" min="19" style="0" width="16.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="13.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="13.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="15.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="15.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="88.63"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4553,31 +4650,37 @@
       <c r="V1" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D2" s="3" t="n">
         <v>1</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="I2" s="0" t="n">
         <v>1000</v>
@@ -4597,29 +4700,37 @@
       <c r="N2" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="O2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="P2" s="5" t="s">
-        <v>29</v>
+      <c r="O2" s="4" t="n">
+        <f aca="false">J2/('Lab Modules'!G3*3600)</f>
+        <v>50.0000014</v>
+      </c>
+      <c r="P2" s="4" t="n">
+        <f aca="false">O2/4</f>
+        <v>12.50000035</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="R2" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="S2" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="T2" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="U2" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
+      </c>
+      <c r="R2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="S2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="T2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="U2" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="V2" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
+      </c>
+      <c r="W2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="X2" s="7" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4627,25 +4738,25 @@
         <v>13</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D3" s="3" t="n">
         <v>1</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="I3" s="0" t="n">
         <v>1000</v>
@@ -4665,89 +4776,99 @@
       <c r="N3" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="O3" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="P3" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q3" s="7"/>
-      <c r="R3" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="S3" s="7" t="s">
-        <v>29</v>
-      </c>
+      <c r="O3" s="4" t="n">
+        <f aca="false">N3/('Lab Modules'!G9*3600)</f>
+        <v>50.0000014</v>
+      </c>
+      <c r="P3" s="4" t="n">
+        <f aca="false">O3/4</f>
+        <v>12.50000035</v>
+      </c>
+      <c r="Q3" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="R3" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="S3" s="8"/>
       <c r="T3" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="U3" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="V3" s="6" t="s">
-        <v>37</v>
+        <v>31</v>
+      </c>
+      <c r="U3" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="V3" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="W3" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="X3" s="7" t="s">
+        <v>39</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>19</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="10" t="n">
+      <c r="B4" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="10"/>
+      <c r="D4" s="11" t="n">
         <v>1</v>
       </c>
-      <c r="E4" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9" t="s">
+      <c r="E4" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9" t="n">
+      <c r="F4" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10" t="n">
         <v>50</v>
       </c>
-      <c r="K4" s="9" t="n">
+      <c r="K4" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="L4" s="9" t="n">
+      <c r="L4" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="M4" s="9" t="n">
+      <c r="M4" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="N4" s="9" t="n">
+      <c r="N4" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="O4" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="P4" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q4" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="R4" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="S4" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="T4" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="U4" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="V4" s="0" t="s">
-        <v>42</v>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="R4" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="S4" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="T4" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="U4" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="V4" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="W4" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="X4" s="15" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4755,25 +4876,25 @@
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D5" s="3" t="n">
         <v>1</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G5" s="0" t="s">
         <v>10</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="I5" s="0" t="n">
         <v>1100</v>
@@ -4793,29 +4914,37 @@
       <c r="N5" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="O5" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="P5" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q5" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="R5" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="S5" s="5" t="s">
-        <v>29</v>
+      <c r="O5" s="16" t="n">
+        <f aca="false">K5/('Lab Modules'!G7*3600)</f>
+        <v>0.0138888888888889</v>
+      </c>
+      <c r="P5" s="4" t="n">
+        <f aca="false">O5/4</f>
+        <v>0.00347222222222222</v>
+      </c>
+      <c r="Q5" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="R5" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="S5" s="14" t="s">
+        <v>31</v>
       </c>
       <c r="T5" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="U5" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
+      </c>
+      <c r="U5" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="V5" s="6" t="s">
-        <v>48</v>
+        <v>31</v>
+      </c>
+      <c r="W5" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="X5" s="7" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4823,25 +4952,25 @@
         <v>8</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D6" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="E6" s="14" t="s">
-        <v>51</v>
+      <c r="E6" s="17" t="s">
+        <v>53</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="I6" s="0" t="n">
         <v>1000</v>
@@ -4861,53 +4990,61 @@
       <c r="N6" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="O6" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="P6" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q6" s="13" t="s">
-        <v>29</v>
+      <c r="O6" s="18" t="n">
+        <f aca="false">M6/('Lab Modules'!G5*3600)</f>
+        <v>25.0000007</v>
+      </c>
+      <c r="P6" s="4" t="n">
+        <f aca="false">O6/4</f>
+        <v>6.25000017500001</v>
+      </c>
+      <c r="Q6" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="R6" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="S6" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="T6" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="U6" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
+      </c>
+      <c r="S6" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="T6" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="U6" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="V6" s="6" t="s">
-        <v>55</v>
+        <v>31</v>
+      </c>
+      <c r="W6" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="X6" s="7" t="s">
+        <v>57</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>14</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="3" t="n">
         <v>2</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="I7" s="0" t="n">
         <v>1100</v>
@@ -4927,241 +5064,247 @@
       <c r="N7" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="O7" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="P7" s="5" t="s">
-        <v>29</v>
-      </c>
       <c r="Q7" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="R7" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="S7" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="T7" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="U7" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="V7" s="6" t="s">
-        <v>58</v>
+        <v>30</v>
+      </c>
+      <c r="R7" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="S7" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="T7" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="U7" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="V7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="W7" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="X7" s="7" t="s">
+        <v>60</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="B8" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="10" t="n">
+      <c r="B8" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" s="10"/>
+      <c r="D8" s="11" t="n">
         <v>2</v>
       </c>
-      <c r="E8" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9" t="n">
+      <c r="E8" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10" t="n">
         <v>100</v>
       </c>
-      <c r="K8" s="9" t="n">
+      <c r="K8" s="10" t="n">
         <v>50</v>
       </c>
-      <c r="L8" s="9" t="n">
+      <c r="L8" s="10" t="n">
         <v>20</v>
       </c>
-      <c r="M8" s="9" t="n">
+      <c r="M8" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="N8" s="9" t="n">
+      <c r="N8" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="O8" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="P8" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q8" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="R8" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="S8" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="T8" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="U8" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="V8" s="0" t="s">
-        <v>61</v>
+      <c r="O8" s="10"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="R8" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="S8" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="T8" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="U8" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="V8" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="W8" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="X8" s="15" t="s">
+        <v>63</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
         <v>21</v>
       </c>
-      <c r="B9" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="10" t="n">
+      <c r="B9" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="10"/>
+      <c r="D9" s="11" t="n">
         <v>2</v>
       </c>
-      <c r="E9" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9" t="n">
+      <c r="E9" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10" t="n">
         <v>100</v>
       </c>
-      <c r="K9" s="9" t="n">
+      <c r="K9" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="L9" s="9" t="n">
+      <c r="L9" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="M9" s="9" t="n">
+      <c r="M9" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="N9" s="9" t="n">
+      <c r="N9" s="10" t="n">
         <v>50</v>
       </c>
-      <c r="O9" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="P9" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q9" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="R9" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="S9" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="T9" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="U9" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="V9" s="0" t="s">
-        <v>64</v>
+      <c r="O9" s="10"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="R9" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="S9" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="T9" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="U9" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="V9" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="W9" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="X9" s="15" t="s">
+        <v>66</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="B10" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="10" t="n">
+      <c r="B10" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10" s="10"/>
+      <c r="D10" s="11" t="n">
         <v>2</v>
       </c>
-      <c r="E10" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9" t="n">
+      <c r="E10" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10" t="n">
         <v>100</v>
       </c>
-      <c r="K10" s="9" t="n">
+      <c r="K10" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="L10" s="9" t="n">
+      <c r="L10" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="M10" s="9" t="n">
+      <c r="M10" s="10" t="n">
         <v>50</v>
       </c>
-      <c r="N10" s="9" t="n">
+      <c r="N10" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="O10" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="P10" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q10" s="13" t="s">
-        <v>29</v>
+      <c r="O10" s="10"/>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="12" t="s">
+        <v>30</v>
       </c>
       <c r="R10" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="S10" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="T10" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="U10" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="V10" s="0" t="s">
-        <v>67</v>
+        <v>30</v>
+      </c>
+      <c r="S10" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="T10" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="U10" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="V10" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="W10" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="X10" s="15" t="s">
+        <v>69</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
         <v>3</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D11" s="3" t="n">
         <v>2</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G11" s="0" t="s">
         <v>10</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="I11" s="0" t="n">
         <v>1200</v>
@@ -5181,55 +5324,55 @@
       <c r="N11" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="O11" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="P11" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q11" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="R11" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="S11" s="5" t="s">
-        <v>29</v>
+      <c r="Q11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="R11" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="S11" s="14" t="s">
+        <v>31</v>
       </c>
       <c r="T11" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="U11" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
+      </c>
+      <c r="U11" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="V11" s="6" t="s">
-        <v>72</v>
+        <v>31</v>
+      </c>
+      <c r="W11" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="X11" s="7" t="s">
+        <v>74</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <v>5</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D12" s="3" t="n">
         <v>2</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="I12" s="0" t="n">
         <v>1200</v>
@@ -5249,55 +5392,55 @@
       <c r="N12" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="O12" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="P12" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q12" s="13" t="s">
-        <v>29</v>
+      <c r="Q12" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="R12" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="S12" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="T12" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="U12" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
+      </c>
+      <c r="S12" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="T12" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="U12" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="V12" s="6" t="s">
-        <v>76</v>
+        <v>31</v>
+      </c>
+      <c r="W12" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="X12" s="7" t="s">
+        <v>78</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
         <v>7</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D13" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="E13" s="14" t="s">
-        <v>79</v>
+      <c r="E13" s="17" t="s">
+        <v>81</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="I13" s="0" t="n">
         <v>1000</v>
@@ -5317,53 +5460,53 @@
       <c r="N13" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="O13" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="P13" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q13" s="13" t="s">
-        <v>29</v>
+      <c r="Q13" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="R13" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="S13" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="T13" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="U13" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
+      </c>
+      <c r="S13" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="T13" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="U13" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="V13" s="6" t="s">
-        <v>80</v>
+        <v>31</v>
+      </c>
+      <c r="W13" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="X13" s="7" t="s">
+        <v>82</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
         <v>15</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="3" t="n">
         <v>3</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="I14" s="0" t="n">
         <v>1300</v>
@@ -5383,51 +5526,51 @@
       <c r="N14" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="O14" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="P14" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q14" s="7"/>
-      <c r="R14" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="S14" s="7" t="s">
-        <v>29</v>
-      </c>
+      <c r="Q14" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="R14" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="S14" s="8"/>
       <c r="T14" s="8" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="U14" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="V14" s="6" t="s">
-        <v>83</v>
+        <v>31</v>
+      </c>
+      <c r="V14" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="W14" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="X14" s="7" t="s">
+        <v>85</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
         <v>17</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="3" t="n">
         <v>3</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="I15" s="0" t="n">
         <v>1500</v>
@@ -5447,51 +5590,51 @@
       <c r="N15" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="O15" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="P15" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q15" s="17"/>
-      <c r="R15" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="S15" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="T15" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="U15" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="V15" s="6" t="s">
-        <v>87</v>
+      <c r="Q15" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="R15" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="S15" s="21"/>
+      <c r="T15" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="U15" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="V15" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="W15" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="X15" s="7" t="s">
+        <v>89</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
         <v>18</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="3" t="n">
         <v>3</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="I16" s="0" t="n">
         <v>1500</v>
@@ -5511,53 +5654,53 @@
       <c r="N16" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="O16" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="P16" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q16" s="17"/>
-      <c r="R16" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="S16" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="T16" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="U16" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="V16" s="6" t="s">
-        <v>91</v>
+      <c r="Q16" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="R16" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="S16" s="21"/>
+      <c r="T16" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="U16" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="V16" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="W16" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="X16" s="7" t="s">
+        <v>93</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
         <v>4</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D17" s="3" t="n">
         <v>3</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G17" s="0" t="s">
         <v>10</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="I17" s="0" t="n">
         <v>1500</v>
@@ -5577,55 +5720,55 @@
       <c r="N17" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="O17" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="P17" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q17" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="R17" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="S17" s="4" t="s">
-        <v>28</v>
+      <c r="Q17" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="R17" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="S17" s="14" t="s">
+        <v>31</v>
       </c>
       <c r="T17" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="U17" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="V17" s="6" t="s">
-        <v>96</v>
+        <v>31</v>
+      </c>
+      <c r="W17" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="X17" s="7" t="s">
+        <v>98</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
         <v>6</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D18" s="3" t="n">
         <v>3</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="I18" s="0" t="n">
         <v>1500</v>
@@ -5645,55 +5788,55 @@
       <c r="N18" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="O18" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="P18" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q18" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="R18" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="S18" s="5" t="s">
-        <v>29</v>
+      <c r="Q18" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="R18" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="S18" s="14" t="s">
+        <v>31</v>
       </c>
       <c r="T18" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="U18" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
+      </c>
+      <c r="U18" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="V18" s="6" t="s">
-        <v>101</v>
+        <v>31</v>
+      </c>
+      <c r="W18" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="X18" s="7" t="s">
+        <v>103</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
         <v>9</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D19" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="E19" s="14" t="s">
-        <v>104</v>
+      <c r="E19" s="17" t="s">
+        <v>106</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="I19" s="0" t="n">
         <v>1500</v>
@@ -5713,53 +5856,53 @@
       <c r="N19" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="O19" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="P19" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q19" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="R19" s="4" t="s">
-        <v>28</v>
+      <c r="Q19" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="R19" s="22" t="s">
+        <v>30</v>
       </c>
       <c r="S19" s="19" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="T19" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="U19" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
+      </c>
+      <c r="U19" s="23" t="s">
+        <v>31</v>
       </c>
       <c r="V19" s="6" t="s">
-        <v>106</v>
+        <v>31</v>
+      </c>
+      <c r="W19" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="X19" s="7" t="s">
+        <v>108</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
         <v>10</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="E20" s="20" t="s">
-        <v>108</v>
+      <c r="E20" s="24" t="s">
+        <v>110</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="I20" s="0" t="n">
         <v>3000</v>
@@ -5779,51 +5922,51 @@
       <c r="N20" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="O20" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="P20" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q20" s="8"/>
-      <c r="R20" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="S20" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="T20" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="U20" s="5" t="s">
-        <v>29</v>
+      <c r="Q20" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="R20" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="S20" s="9"/>
+      <c r="T20" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="U20" s="9" t="s">
+        <v>30</v>
       </c>
       <c r="V20" s="6" t="s">
-        <v>111</v>
+        <v>31</v>
+      </c>
+      <c r="W20" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="X20" s="7" t="s">
+        <v>113</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
         <v>11</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="3" t="n">
         <v>4</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="I21" s="0" t="n">
         <v>3000</v>
@@ -5843,53 +5986,53 @@
       <c r="N21" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="O21" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="P21" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q21" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="R21" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="S21" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="T21" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="U21" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="V21" s="6" t="s">
-        <v>114</v>
+      <c r="Q21" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="R21" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="S21" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="T21" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="U21" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="V21" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="W21" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="X21" s="7" t="s">
+        <v>116</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
         <v>12</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="3" t="n">
         <v>4</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="I22" s="0" t="n">
         <v>3000</v>
@@ -5909,53 +6052,53 @@
       <c r="N22" s="0" t="n">
         <v>150</v>
       </c>
-      <c r="O22" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="P22" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q22" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="R22" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="S22" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="T22" s="4" t="s">
-        <v>28</v>
+      <c r="Q22" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="R22" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="S22" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="T22" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="U22" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="V22" s="6" t="s">
-        <v>117</v>
+        <v>30</v>
+      </c>
+      <c r="V22" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="W22" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="X22" s="7" t="s">
+        <v>119</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
         <v>16</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="3" t="n">
         <v>4</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="I23" s="0" t="n">
         <v>3000</v>
@@ -5975,27 +6118,27 @@
       <c r="N23" s="0" t="n">
         <v>500</v>
       </c>
-      <c r="O23" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="P23" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q23" s="8"/>
+      <c r="Q23" s="9" t="s">
+        <v>30</v>
+      </c>
       <c r="R23" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="S23" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="T23" s="8" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+      <c r="S23" s="9"/>
+      <c r="T23" s="9" t="s">
+        <v>30</v>
       </c>
       <c r="U23" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="V23" s="6" t="s">
-        <v>120</v>
+        <v>31</v>
+      </c>
+      <c r="V23" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="W23" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="X23" s="7" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6003,16 +6146,16 @@
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G63" s="0" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="H63" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J63" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="K63" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="L63" s="0" t="n">
         <v>100</v>
@@ -6020,32 +6163,46 @@
       <c r="M63" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="O63" s="0" t="n">
+      <c r="Q63" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="P63" s="0" t="n">
+      <c r="R63" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="R63" s="0" t="s">
-        <v>123</v>
+      <c r="T63" s="0" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G64" s="0" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="H64" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J64" s="0" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="K64" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:V23"/>
+  <autoFilter ref="A1:X23">
+    <filterColumn colId="5">
+      <filters>
+        <filter val="Biology"/>
+        <filter val="Chemistry"/>
+        <filter val="Physics"/>
+        <filter val="Physiology"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="3">
+      <filters>
+        <filter val="1"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -6069,7 +6226,7 @@
       <selection pane="topLeft" activeCell="G27" activeCellId="0" sqref="G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.69"/>
@@ -6080,101 +6237,101 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="21"/>
-      <c r="B1" s="22" t="s">
-        <v>126</v>
-      </c>
-      <c r="C1" s="22" t="s">
-        <v>127</v>
-      </c>
-      <c r="D1" s="22" t="s">
+      <c r="A1" s="25"/>
+      <c r="B1" s="26" t="s">
         <v>128</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="C1" s="26" t="s">
         <v>129</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="D1" s="26" t="s">
         <v>130</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="E1" s="26" t="s">
         <v>131</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>132</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="23" t="s">
-        <v>132</v>
-      </c>
-      <c r="B2" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="D2" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="E2" s="27" t="s">
-        <v>133</v>
-      </c>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
+      <c r="A2" s="27" t="s">
+        <v>134</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="31" t="s">
+        <v>135</v>
+      </c>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="23" t="s">
-        <v>134</v>
-      </c>
-      <c r="B3" s="28" t="s">
-        <v>79</v>
-      </c>
-      <c r="C3" s="29" t="s">
-        <v>75</v>
-      </c>
-      <c r="D3" s="26" t="s">
-        <v>70</v>
-      </c>
-      <c r="E3" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
+      <c r="A3" s="27" t="s">
+        <v>136</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="E3" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="30" t="s">
-        <v>135</v>
-      </c>
-      <c r="B4" s="31" t="s">
-        <v>136</v>
-      </c>
-      <c r="C4" s="32" t="s">
+      <c r="A4" s="34" t="s">
         <v>137</v>
       </c>
-      <c r="D4" s="33" t="s">
-        <v>94</v>
-      </c>
-      <c r="E4" s="34" t="s">
-        <v>82</v>
-      </c>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
+      <c r="B4" s="35" t="s">
+        <v>138</v>
+      </c>
+      <c r="C4" s="36" t="s">
+        <v>139</v>
+      </c>
+      <c r="D4" s="37" t="s">
+        <v>96</v>
+      </c>
+      <c r="E4" s="38" t="s">
+        <v>84</v>
+      </c>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="23" t="s">
-        <v>138</v>
-      </c>
-      <c r="B5" s="35" t="s">
-        <v>108</v>
-      </c>
-      <c r="C5" s="35" t="s">
-        <v>139</v>
-      </c>
-      <c r="D5" s="35" t="s">
-        <v>116</v>
-      </c>
-      <c r="E5" s="35" t="s">
+      <c r="A5" s="27" t="s">
         <v>140</v>
       </c>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
+      <c r="B5" s="39" t="s">
+        <v>110</v>
+      </c>
+      <c r="C5" s="39" t="s">
+        <v>141</v>
+      </c>
+      <c r="D5" s="39" t="s">
+        <v>118</v>
+      </c>
+      <c r="E5" s="39" t="s">
+        <v>142</v>
+      </c>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -6193,25 +6350,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F25" activeCellId="0" sqref="F25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F26" activeCellId="0" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="19.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="15.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="0" width="20.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="131.85"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -6220,322 +6376,321 @@
         <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="36" t="s">
-        <v>146</v>
-      </c>
-      <c r="B2" s="36" t="s">
-        <v>147</v>
-      </c>
-      <c r="C2" s="36" t="s">
+      <c r="A2" s="40" t="s">
         <v>148</v>
       </c>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37" t="s">
+      <c r="B2" s="40" t="s">
         <v>149</v>
       </c>
-      <c r="F2" s="38" t="s">
+      <c r="C2" s="40" t="s">
         <v>150</v>
       </c>
-      <c r="G2" s="37" t="s">
+      <c r="D2" s="41"/>
+      <c r="E2" s="41" t="s">
+        <v>151</v>
+      </c>
+      <c r="F2" s="42" t="s">
+        <v>152</v>
+      </c>
+      <c r="G2" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="39" t="s">
-        <v>151</v>
+      <c r="H2" s="43" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="36"/>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37" t="n">
+      <c r="A3" s="40"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41" t="n">
         <v>6.25</v>
       </c>
-      <c r="F3" s="38" t="s">
-        <v>150</v>
-      </c>
-      <c r="G3" s="37" t="n">
+      <c r="F3" s="42" t="s">
+        <v>152</v>
+      </c>
+      <c r="G3" s="41" t="n">
         <v>0.00027777777</v>
       </c>
-      <c r="H3" s="39"/>
+      <c r="H3" s="43"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="40" t="s">
-        <v>152</v>
-      </c>
-      <c r="B4" s="40" t="s">
-        <v>153</v>
-      </c>
-      <c r="C4" s="40" t="s">
+      <c r="A4" s="44" t="s">
         <v>154</v>
       </c>
-      <c r="D4" s="41" t="s">
+      <c r="B4" s="44" t="s">
         <v>155</v>
       </c>
-      <c r="E4" s="41" t="s">
-        <v>149</v>
-      </c>
-      <c r="F4" s="41" t="s">
-        <v>155</v>
-      </c>
-      <c r="G4" s="41" t="s">
+      <c r="C4" s="44" t="s">
         <v>156</v>
       </c>
-      <c r="H4" s="42" t="s">
+      <c r="D4" s="45" t="s">
         <v>157</v>
+      </c>
+      <c r="E4" s="45" t="s">
+        <v>151</v>
+      </c>
+      <c r="F4" s="45" t="s">
+        <v>157</v>
+      </c>
+      <c r="G4" s="45" t="s">
+        <v>158</v>
+      </c>
+      <c r="H4" s="46" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="40"/>
-      <c r="B5" s="40"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="41" t="n">
+      <c r="A5" s="44"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="45" t="n">
         <v>50</v>
       </c>
-      <c r="E5" s="41" t="n">
+      <c r="E5" s="45" t="n">
         <v>0.00138888888</v>
       </c>
-      <c r="F5" s="41" t="n">
+      <c r="F5" s="45" t="n">
         <v>0.00027777777</v>
       </c>
-      <c r="G5" s="41" t="n">
+      <c r="G5" s="45" t="n">
         <v>0.00027777777</v>
       </c>
-      <c r="H5" s="42"/>
+      <c r="H5" s="46"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="43" t="s">
-        <v>158</v>
-      </c>
-      <c r="B6" s="43" t="s">
-        <v>159</v>
-      </c>
-      <c r="C6" s="43" t="s">
+      <c r="A6" s="47" t="s">
         <v>160</v>
       </c>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44" t="s">
-        <v>149</v>
-      </c>
-      <c r="F6" s="45" t="s">
-        <v>150</v>
-      </c>
-      <c r="G6" s="44" t="s">
+      <c r="B6" s="47" t="s">
+        <v>161</v>
+      </c>
+      <c r="C6" s="47" t="s">
+        <v>162</v>
+      </c>
+      <c r="D6" s="48"/>
+      <c r="E6" s="48" t="s">
+        <v>151</v>
+      </c>
+      <c r="F6" s="49" t="s">
+        <v>152</v>
+      </c>
+      <c r="G6" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="46" t="s">
-        <v>161</v>
+      <c r="H6" s="50" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="43"/>
-      <c r="B7" s="43"/>
-      <c r="C7" s="43"/>
-      <c r="D7" s="44"/>
-      <c r="E7" s="44" t="n">
+      <c r="A7" s="47"/>
+      <c r="B7" s="47"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="48"/>
+      <c r="E7" s="48" t="n">
         <v>90</v>
       </c>
-      <c r="F7" s="45" t="s">
-        <v>150</v>
-      </c>
-      <c r="G7" s="44" t="n">
+      <c r="F7" s="49" t="s">
+        <v>152</v>
+      </c>
+      <c r="G7" s="48" t="n">
         <v>1</v>
       </c>
-      <c r="H7" s="46"/>
+      <c r="H7" s="50"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="47" t="s">
-        <v>162</v>
-      </c>
-      <c r="B8" s="47" t="s">
-        <v>163</v>
-      </c>
-      <c r="C8" s="47" t="s">
+      <c r="A8" s="51" t="s">
         <v>164</v>
       </c>
-      <c r="D8" s="48" t="s">
-        <v>35</v>
-      </c>
-      <c r="E8" s="48" t="s">
-        <v>149</v>
-      </c>
-      <c r="F8" s="48" t="s">
-        <v>35</v>
-      </c>
-      <c r="G8" s="48" t="s">
+      <c r="B8" s="51" t="s">
+        <v>165</v>
+      </c>
+      <c r="C8" s="51" t="s">
+        <v>166</v>
+      </c>
+      <c r="D8" s="52" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="52" t="s">
+        <v>151</v>
+      </c>
+      <c r="F8" s="52" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="49" t="s">
-        <v>165</v>
+      <c r="H8" s="53" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="47"/>
-      <c r="B9" s="47"/>
-      <c r="C9" s="47"/>
-      <c r="D9" s="48" t="n">
+      <c r="A9" s="51"/>
+      <c r="B9" s="51"/>
+      <c r="C9" s="51"/>
+      <c r="D9" s="52" t="n">
         <v>300</v>
       </c>
-      <c r="E9" s="48" t="n">
+      <c r="E9" s="52" t="n">
         <v>0.00138888888</v>
       </c>
-      <c r="F9" s="48" t="n">
+      <c r="F9" s="52" t="n">
         <v>0.00138888888</v>
       </c>
-      <c r="G9" s="48" t="n">
+      <c r="G9" s="52" t="n">
         <v>0.00027777777</v>
       </c>
-      <c r="H9" s="49"/>
+      <c r="H9" s="53"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="50" t="s">
-        <v>166</v>
-      </c>
-      <c r="B10" s="50" t="s">
-        <v>167</v>
-      </c>
-      <c r="C10" s="50" t="s">
+      <c r="A10" s="54" t="s">
         <v>168</v>
       </c>
-      <c r="D10" s="51"/>
-      <c r="E10" s="52" t="s">
-        <v>149</v>
-      </c>
-      <c r="F10" s="52" t="s">
+      <c r="B10" s="54" t="s">
+        <v>169</v>
+      </c>
+      <c r="C10" s="54" t="s">
+        <v>170</v>
+      </c>
+      <c r="D10" s="55"/>
+      <c r="E10" s="56" t="s">
+        <v>151</v>
+      </c>
+      <c r="F10" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="52" t="s">
-        <v>169</v>
-      </c>
-      <c r="H10" s="53"/>
+      <c r="G10" s="56" t="s">
+        <v>171</v>
+      </c>
+      <c r="H10" s="57"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="50"/>
-      <c r="B11" s="50"/>
-      <c r="C11" s="50"/>
-      <c r="D11" s="51"/>
-      <c r="E11" s="52" t="s">
-        <v>170</v>
-      </c>
-      <c r="F11" s="52"/>
-      <c r="G11" s="52" t="s">
-        <v>170</v>
-      </c>
-      <c r="H11" s="53"/>
+      <c r="A11" s="54"/>
+      <c r="B11" s="54"/>
+      <c r="C11" s="54"/>
+      <c r="D11" s="55"/>
+      <c r="E11" s="56" t="s">
+        <v>172</v>
+      </c>
+      <c r="F11" s="56"/>
+      <c r="G11" s="56" t="s">
+        <v>172</v>
+      </c>
+      <c r="H11" s="57"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="54" t="s">
-        <v>171</v>
-      </c>
-      <c r="B12" s="54" t="s">
-        <v>172</v>
-      </c>
-      <c r="C12" s="54" t="s">
+      <c r="A12" s="58" t="s">
         <v>173</v>
       </c>
-      <c r="D12" s="55"/>
-      <c r="E12" s="55" t="s">
+      <c r="B12" s="58" t="s">
         <v>174</v>
       </c>
-      <c r="F12" s="55"/>
-      <c r="G12" s="55"/>
-      <c r="H12" s="56" t="s">
+      <c r="C12" s="58" t="s">
         <v>175</v>
+      </c>
+      <c r="D12" s="59"/>
+      <c r="E12" s="59" t="s">
+        <v>176</v>
+      </c>
+      <c r="F12" s="59"/>
+      <c r="G12" s="59"/>
+      <c r="H12" s="60" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="54"/>
-      <c r="B13" s="54"/>
-      <c r="C13" s="54"/>
-      <c r="D13" s="55"/>
-      <c r="E13" s="55" t="s">
-        <v>176</v>
-      </c>
-      <c r="F13" s="55"/>
-      <c r="G13" s="55"/>
-      <c r="H13" s="56"/>
+      <c r="A13" s="58"/>
+      <c r="B13" s="58"/>
+      <c r="C13" s="58"/>
+      <c r="D13" s="59"/>
+      <c r="E13" s="59" t="s">
+        <v>178</v>
+      </c>
+      <c r="F13" s="59"/>
+      <c r="G13" s="59"/>
+      <c r="H13" s="60"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="57" t="s">
-        <v>177</v>
-      </c>
-      <c r="B14" s="58" t="s">
-        <v>178</v>
-      </c>
-      <c r="C14" s="57" t="s">
+      <c r="A14" s="61" t="s">
         <v>179</v>
       </c>
-      <c r="D14" s="59" t="s">
-        <v>155</v>
-      </c>
-      <c r="E14" s="59"/>
-      <c r="F14" s="59"/>
-      <c r="G14" s="59"/>
-      <c r="H14" s="60" t="s">
+      <c r="B14" s="62" t="s">
         <v>180</v>
+      </c>
+      <c r="C14" s="61" t="s">
+        <v>181</v>
+      </c>
+      <c r="D14" s="63" t="s">
+        <v>157</v>
+      </c>
+      <c r="E14" s="63"/>
+      <c r="F14" s="63"/>
+      <c r="G14" s="63"/>
+      <c r="H14" s="64" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="57"/>
-      <c r="B15" s="57"/>
-      <c r="C15" s="57"/>
-      <c r="D15" s="59" t="n">
+      <c r="A15" s="61"/>
+      <c r="B15" s="61"/>
+      <c r="C15" s="61"/>
+      <c r="D15" s="63" t="n">
         <v>100</v>
       </c>
-      <c r="E15" s="59"/>
-      <c r="F15" s="59"/>
-      <c r="G15" s="59"/>
-      <c r="H15" s="60"/>
+      <c r="E15" s="63"/>
+      <c r="F15" s="63"/>
+      <c r="G15" s="63"/>
+      <c r="H15" s="64"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="58" t="s">
-        <v>181</v>
-      </c>
-      <c r="B16" s="58" t="s">
-        <v>181</v>
-      </c>
-      <c r="C16" s="57" t="s">
-        <v>182</v>
-      </c>
-      <c r="D16" s="59" t="s">
-        <v>155</v>
-      </c>
-      <c r="E16" s="59"/>
-      <c r="F16" s="59"/>
-      <c r="G16" s="59"/>
-      <c r="H16" s="60" t="s">
+      <c r="A16" s="62" t="s">
         <v>183</v>
+      </c>
+      <c r="B16" s="62" t="s">
+        <v>183</v>
+      </c>
+      <c r="C16" s="61" t="s">
+        <v>184</v>
+      </c>
+      <c r="D16" s="63" t="s">
+        <v>157</v>
+      </c>
+      <c r="E16" s="63"/>
+      <c r="F16" s="63"/>
+      <c r="G16" s="63"/>
+      <c r="H16" s="64" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="58"/>
-      <c r="B17" s="58"/>
-      <c r="C17" s="58"/>
-      <c r="D17" s="59" t="n">
+      <c r="A17" s="62"/>
+      <c r="B17" s="62"/>
+      <c r="C17" s="62"/>
+      <c r="D17" s="63" t="n">
         <v>30</v>
       </c>
-      <c r="E17" s="59"/>
-      <c r="F17" s="59"/>
-      <c r="G17" s="59"/>
-      <c r="H17" s="60"/>
+      <c r="E17" s="63"/>
+      <c r="F17" s="63"/>
+      <c r="G17" s="63"/>
+      <c r="H17" s="64"/>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <autoFilter ref="A1:G11"/>
   <mergeCells count="32">

</xml_diff>

<commit_message>
minor tweaks and excel update
</commit_message>
<xml_diff>
--- a/Docs/Station Science List.xlsx
+++ b/Docs/Station Science List.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Experiments and Notes" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Tech Tree and To-Do" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Lab Modules" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Conversion Rates" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Experiments and Notes'!$A$1:$X$23</definedName>
@@ -51,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="191">
   <si>
     <t xml:space="preserve">Experiment No.:</t>
   </si>
@@ -868,6 +869,21 @@
   </si>
   <si>
     <t xml:space="preserve">All the features of our classic Kibbal Storage, now in Fun Size! </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit per Hour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">per second</t>
+  </si>
+  <si>
+    <t xml:space="preserve">per minute</t>
+  </si>
+  <si>
+    <t xml:space="preserve">per hour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">per Kerbin day</t>
   </si>
 </sst>
 </file>
@@ -1247,7 +1263,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="66">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1508,6 +1524,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="16">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4374,13 +4394,13 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1028520</xdr:colOff>
+      <xdr:colOff>959760</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>25560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>5839200</xdr:colOff>
+      <xdr:colOff>5770440</xdr:colOff>
       <xdr:row>38</xdr:row>
       <xdr:rowOff>39600</xdr:rowOff>
     </xdr:to>
@@ -4391,7 +4411,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9162360" y="3706200"/>
+          <a:off x="9093600" y="3706200"/>
           <a:ext cx="6234840" cy="2993400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4550,10 +4570,10 @@
   </sheetPr>
   <dimension ref="A1:X64"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="4" ySplit="0" topLeftCell="E1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="P31" activeCellId="0" sqref="P31"/>
+      <selection pane="topRight" activeCell="N25" activeCellId="0" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.01953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6736,4 +6756,933 @@
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E50"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H17" activeCellId="0" sqref="H17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.65"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B11" s="65" t="n">
+        <v>0.00027777777</v>
+      </c>
+      <c r="C11" s="65" t="n">
+        <v>0.0166666662</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>0.999999972</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>3.999999888</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <f aca="false">B11*A12</f>
+        <v>0.00055555554</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <f aca="false">C11*A12</f>
+        <v>0.0333333324</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <f aca="false">D11*A12</f>
+        <v>1.999999944</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <f aca="false">E11*A12</f>
+        <v>7.999999776</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <f aca="false">B12*A13</f>
+        <v>0.00166666662</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <f aca="false">C12*A13</f>
+        <v>0.0999999972</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <f aca="false">D12*A13</f>
+        <v>5.999999832</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <f aca="false">E12*A13</f>
+        <v>23.999999328</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <f aca="false">B13*A14</f>
+        <v>0.00666666648</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <f aca="false">C13*A14</f>
+        <v>0.3999999888</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <f aca="false">D13*A14</f>
+        <v>23.999999328</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <f aca="false">E13*A14</f>
+        <v>95.999997312</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <f aca="false">B14*A15</f>
+        <v>0.0333333324</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <f aca="false">C14*A15</f>
+        <v>1.999999944</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <f aca="false">D14*A15</f>
+        <v>119.99999664</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <f aca="false">E14*A15</f>
+        <v>479.99998656</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <f aca="false">B15*A16</f>
+        <v>0.1999999944</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <f aca="false">C15*A16</f>
+        <v>11.999999664</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <f aca="false">D15*A16</f>
+        <v>719.99997984</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <f aca="false">E15*A16</f>
+        <v>2879.99991936</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <f aca="false">B16*A17</f>
+        <v>1.3999999608</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <f aca="false">C16*A17</f>
+        <v>83.999997648</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <f aca="false">D16*A17</f>
+        <v>5039.99985888</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <f aca="false">E16*A17</f>
+        <v>20159.99943552</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <f aca="false">B17*A18</f>
+        <v>11.1999996864</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <f aca="false">C17*A18</f>
+        <v>671.999981184</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <f aca="false">D17*A18</f>
+        <v>40319.99887104</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <f aca="false">E17*A18</f>
+        <v>161279.99548416</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <f aca="false">B18*A19</f>
+        <v>100.7999971776</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <f aca="false">C18*A19</f>
+        <v>6047.999830656</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <f aca="false">D18*A19</f>
+        <v>362879.98983936</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <f aca="false">E18*A19</f>
+        <v>1451519.95935744</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <f aca="false">B19*A20</f>
+        <v>1007.999971776</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <f aca="false">C19*A20</f>
+        <v>60479.99830656</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <f aca="false">D19*A20</f>
+        <v>3628799.8983936</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <f aca="false">E19*A20</f>
+        <v>14515199.5935744</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <f aca="false">B20*A21</f>
+        <v>11087.999689536</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <f aca="false">C20*A21</f>
+        <v>665279.98137216</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <f aca="false">D20*A21</f>
+        <v>39916798.8823296</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <f aca="false">E20*A21</f>
+        <v>159667195.529318</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <f aca="false">B21*A22</f>
+        <v>133055.996274432</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <f aca="false">C21*A22</f>
+        <v>7983359.77646592</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <f aca="false">D21*A22</f>
+        <v>479001586.587955</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <f aca="false">E21*A22</f>
+        <v>1916006346.35182</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <f aca="false">B22*A23</f>
+        <v>1729727.95156762</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <f aca="false">C22*A23</f>
+        <v>103783677.094057</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <f aca="false">D22*A23</f>
+        <v>6227020625.64342</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <f aca="false">E22*A23</f>
+        <v>24908082502.5737</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <f aca="false">B23*A24</f>
+        <v>24216191.3219466</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <f aca="false">C23*A24</f>
+        <v>1452971479.3168</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <f aca="false">D23*A24</f>
+        <v>87178288759.0079</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <f aca="false">E23*A24</f>
+        <v>348713155036.031</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <f aca="false">B24*A25</f>
+        <v>363242869.829199</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <f aca="false">C24*A25</f>
+        <v>21794572189.752</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <f aca="false">D24*A25</f>
+        <v>1307674331385.12</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <f aca="false">E24*A25</f>
+        <v>5230697325540.47</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <f aca="false">B25*A26</f>
+        <v>5811885917.26719</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <f aca="false">C25*A26</f>
+        <v>348713155036.031</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <f aca="false">D25*A26</f>
+        <v>20922789302161.9</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <f aca="false">E25*A26</f>
+        <v>83691157208647.6</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <f aca="false">B26*A27</f>
+        <v>98802060593.5422</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <f aca="false">C26*A27</f>
+        <v>5928123635612.53</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <f aca="false">D26*A27</f>
+        <v>355687418136752</v>
+      </c>
+      <c r="E27" s="0" t="n">
+        <f aca="false">E26*A27</f>
+        <v>1422749672547010</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <f aca="false">B27*A28</f>
+        <v>1778437090683.76</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <f aca="false">C27*A28</f>
+        <v>106706225441026</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <f aca="false">D27*A28</f>
+        <v>6402373526461540</v>
+      </c>
+      <c r="E28" s="0" t="n">
+        <f aca="false">E27*A28</f>
+        <v>25609494105846100</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <f aca="false">B28*A29</f>
+        <v>33790304722991.4</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <f aca="false">C28*A29</f>
+        <v>2027418283379490</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <f aca="false">D28*A29</f>
+        <v>1.21645097002769E+017</v>
+      </c>
+      <c r="E29" s="0" t="n">
+        <f aca="false">E28*A29</f>
+        <v>4.86580388011077E+017</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <f aca="false">B29*A30</f>
+        <v>675806094459829</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <f aca="false">C29*A30</f>
+        <v>40548365667589700</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <f aca="false">D29*A30</f>
+        <v>2.43290194005538E+018</v>
+      </c>
+      <c r="E30" s="0" t="n">
+        <f aca="false">E29*A30</f>
+        <v>9.73160776022154E+018</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <f aca="false">B30*A31</f>
+        <v>14191927983656400</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <f aca="false">C30*A31</f>
+        <v>8.51515679019384E+017</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <f aca="false">D30*A31</f>
+        <v>5.10909407411631E+019</v>
+      </c>
+      <c r="E31" s="0" t="n">
+        <f aca="false">E30*A31</f>
+        <v>2.04363762964652E+020</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <f aca="false">B31*A32</f>
+        <v>3.12222415640441E+017</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <f aca="false">C31*A32</f>
+        <v>1.87333449384265E+019</v>
+      </c>
+      <c r="D32" s="0" t="n">
+        <f aca="false">D31*A32</f>
+        <v>1.12400069630559E+021</v>
+      </c>
+      <c r="E32" s="0" t="n">
+        <f aca="false">E31*A32</f>
+        <v>4.49600278522235E+021</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <f aca="false">B32*A33</f>
+        <v>7.18111555973014E+018</v>
+      </c>
+      <c r="C33" s="0" t="n">
+        <f aca="false">C32*A33</f>
+        <v>4.30866933583808E+020</v>
+      </c>
+      <c r="D33" s="0" t="n">
+        <f aca="false">D32*A33</f>
+        <v>2.58520160150285E+022</v>
+      </c>
+      <c r="E33" s="0" t="n">
+        <f aca="false">E32*A33</f>
+        <v>1.03408064060114E+023</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B34" s="0" t="n">
+        <f aca="false">B33*A34</f>
+        <v>1.72346773433523E+020</v>
+      </c>
+      <c r="C34" s="0" t="n">
+        <f aca="false">C33*A34</f>
+        <v>1.03408064060114E+022</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <f aca="false">D33*A34</f>
+        <v>6.20448384360684E+023</v>
+      </c>
+      <c r="E34" s="0" t="n">
+        <f aca="false">E33*A34</f>
+        <v>2.48179353744274E+024</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <f aca="false">B34*A35</f>
+        <v>4.30866933583808E+021</v>
+      </c>
+      <c r="C35" s="0" t="n">
+        <f aca="false">C34*A35</f>
+        <v>2.58520160150285E+023</v>
+      </c>
+      <c r="D35" s="0" t="n">
+        <f aca="false">D34*A35</f>
+        <v>1.55112096090171E+025</v>
+      </c>
+      <c r="E35" s="0" t="n">
+        <f aca="false">E34*A35</f>
+        <v>6.20448384360684E+025</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <f aca="false">B35*A36</f>
+        <v>1.1202540273179E+023</v>
+      </c>
+      <c r="C36" s="0" t="n">
+        <f aca="false">C35*A36</f>
+        <v>6.72152416390741E+024</v>
+      </c>
+      <c r="D36" s="0" t="n">
+        <f aca="false">D35*A36</f>
+        <v>4.03291449834445E+026</v>
+      </c>
+      <c r="E36" s="0" t="n">
+        <f aca="false">E35*A36</f>
+        <v>1.61316579933778E+027</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B37" s="0" t="n">
+        <f aca="false">B36*A37</f>
+        <v>3.02468587375833E+024</v>
+      </c>
+      <c r="C37" s="0" t="n">
+        <f aca="false">C36*A37</f>
+        <v>1.814811524255E+026</v>
+      </c>
+      <c r="D37" s="0" t="n">
+        <f aca="false">D36*A37</f>
+        <v>1.088886914553E+028</v>
+      </c>
+      <c r="E37" s="0" t="n">
+        <f aca="false">E36*A37</f>
+        <v>4.355547658212E+028</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B38" s="0" t="n">
+        <f aca="false">B37*A38</f>
+        <v>8.46912044652334E+025</v>
+      </c>
+      <c r="C38" s="0" t="n">
+        <f aca="false">C37*A38</f>
+        <v>5.081472267914E+027</v>
+      </c>
+      <c r="D38" s="0" t="n">
+        <f aca="false">D37*A38</f>
+        <v>3.0488833607484E+029</v>
+      </c>
+      <c r="E38" s="0" t="n">
+        <f aca="false">E37*A38</f>
+        <v>1.21955334429936E+030</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B39" s="0" t="n">
+        <f aca="false">B38*A39</f>
+        <v>2.45604492949177E+027</v>
+      </c>
+      <c r="C39" s="0" t="n">
+        <f aca="false">C38*A39</f>
+        <v>1.47362695769506E+029</v>
+      </c>
+      <c r="D39" s="0" t="n">
+        <f aca="false">D38*A39</f>
+        <v>8.84176174617037E+030</v>
+      </c>
+      <c r="E39" s="0" t="n">
+        <f aca="false">E38*A39</f>
+        <v>3.53670469846815E+031</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B40" s="0" t="n">
+        <f aca="false">B39*A40</f>
+        <v>7.3681347884753E+028</v>
+      </c>
+      <c r="C40" s="0" t="n">
+        <f aca="false">C39*A40</f>
+        <v>4.42088087308518E+030</v>
+      </c>
+      <c r="D40" s="0" t="n">
+        <f aca="false">D39*A40</f>
+        <v>2.65252852385111E+032</v>
+      </c>
+      <c r="E40" s="0" t="n">
+        <f aca="false">E39*A40</f>
+        <v>1.06101140954044E+033</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B41" s="0" t="n">
+        <f aca="false">B40*A41</f>
+        <v>2.28412178442734E+030</v>
+      </c>
+      <c r="C41" s="0" t="n">
+        <f aca="false">C40*A41</f>
+        <v>1.37047307065641E+032</v>
+      </c>
+      <c r="D41" s="0" t="n">
+        <f aca="false">D40*A41</f>
+        <v>8.22283842393844E+033</v>
+      </c>
+      <c r="E41" s="0" t="n">
+        <f aca="false">E40*A41</f>
+        <v>3.28913536957538E+034</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B42" s="0" t="n">
+        <f aca="false">B41*A42</f>
+        <v>7.3091897101675E+031</v>
+      </c>
+      <c r="C42" s="0" t="n">
+        <f aca="false">C41*A42</f>
+        <v>4.3855138261005E+033</v>
+      </c>
+      <c r="D42" s="0" t="n">
+        <f aca="false">D41*A42</f>
+        <v>2.6313082956603E+035</v>
+      </c>
+      <c r="E42" s="0" t="n">
+        <f aca="false">E41*A42</f>
+        <v>1.05252331826412E+036</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B43" s="0" t="n">
+        <f aca="false">B42*A43</f>
+        <v>2.41203260435528E+033</v>
+      </c>
+      <c r="C43" s="0" t="n">
+        <f aca="false">C42*A43</f>
+        <v>1.44721956261317E+035</v>
+      </c>
+      <c r="D43" s="0" t="n">
+        <f aca="false">D42*A43</f>
+        <v>8.68331737567899E+036</v>
+      </c>
+      <c r="E43" s="0" t="n">
+        <f aca="false">E42*A43</f>
+        <v>3.4733269502716E+037</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B44" s="0" t="n">
+        <f aca="false">B43*A44</f>
+        <v>8.20091085480794E+034</v>
+      </c>
+      <c r="C44" s="0" t="n">
+        <f aca="false">C43*A44</f>
+        <v>4.92054651288476E+036</v>
+      </c>
+      <c r="D44" s="0" t="n">
+        <f aca="false">D43*A44</f>
+        <v>2.95232790773086E+038</v>
+      </c>
+      <c r="E44" s="0" t="n">
+        <f aca="false">E43*A44</f>
+        <v>1.18093116309234E+039</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B45" s="0" t="n">
+        <f aca="false">B44*A45</f>
+        <v>2.87031879918278E+036</v>
+      </c>
+      <c r="C45" s="0" t="n">
+        <f aca="false">C44*A45</f>
+        <v>1.72219127950967E+038</v>
+      </c>
+      <c r="D45" s="0" t="n">
+        <f aca="false">D44*A45</f>
+        <v>1.0333147677058E+040</v>
+      </c>
+      <c r="E45" s="0" t="n">
+        <f aca="false">E44*A45</f>
+        <v>4.1332590708232E+040</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B46" s="0" t="n">
+        <f aca="false">B45*A46</f>
+        <v>1.0333147677058E+038</v>
+      </c>
+      <c r="C46" s="0" t="n">
+        <f aca="false">C45*A46</f>
+        <v>6.1998886062348E+039</v>
+      </c>
+      <c r="D46" s="0" t="n">
+        <f aca="false">D45*A46</f>
+        <v>3.71993316374088E+041</v>
+      </c>
+      <c r="E46" s="0" t="n">
+        <f aca="false">E45*A46</f>
+        <v>1.48797326549635E+042</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B47" s="0" t="n">
+        <f aca="false">B46*A47</f>
+        <v>3.82326464051146E+039</v>
+      </c>
+      <c r="C47" s="0" t="n">
+        <f aca="false">C46*A47</f>
+        <v>2.29395878430688E+041</v>
+      </c>
+      <c r="D47" s="0" t="n">
+        <f aca="false">D46*A47</f>
+        <v>1.37637527058413E+043</v>
+      </c>
+      <c r="E47" s="0" t="n">
+        <f aca="false">E46*A47</f>
+        <v>5.5055010823365E+043</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B48" s="0" t="n">
+        <f aca="false">B47*A48</f>
+        <v>1.45284056339435E+041</v>
+      </c>
+      <c r="C48" s="0" t="n">
+        <f aca="false">C47*A48</f>
+        <v>8.71704338036613E+042</v>
+      </c>
+      <c r="D48" s="0" t="n">
+        <f aca="false">D47*A48</f>
+        <v>5.23022602821968E+044</v>
+      </c>
+      <c r="E48" s="0" t="n">
+        <f aca="false">E47*A48</f>
+        <v>2.09209041128787E+045</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B49" s="0" t="n">
+        <f aca="false">B48*A49</f>
+        <v>5.66607819723798E+042</v>
+      </c>
+      <c r="C49" s="0" t="n">
+        <f aca="false">C48*A49</f>
+        <v>3.39964691834279E+044</v>
+      </c>
+      <c r="D49" s="0" t="n">
+        <f aca="false">D48*A49</f>
+        <v>2.03978815100567E+046</v>
+      </c>
+      <c r="E49" s="0" t="n">
+        <f aca="false">E48*A49</f>
+        <v>8.1591526040227E+046</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B50" s="0" t="n">
+        <f aca="false">B49*A50</f>
+        <v>2.26643127889519E+044</v>
+      </c>
+      <c r="C50" s="0" t="n">
+        <f aca="false">C49*A50</f>
+        <v>1.35985876733712E+046</v>
+      </c>
+      <c r="D50" s="0" t="n">
+        <f aca="false">D49*A50</f>
+        <v>8.1591526040227E+047</v>
+      </c>
+      <c r="E50" s="0" t="n">
+        <f aca="false">E49*A50</f>
+        <v>3.26366104160908E+048</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>